<commit_message>
Corrected messed up area names in FeFo data
verbatimLocality is set to "Fefo" for all transects in the "FeFo" data. This seems to be an issue with the current version of the data and should be fixed in the database. 
For in the meantime,  I am retrieving the correct area names from the column locationRemarks, and also fixing "Stalluvarre" as being a locality within "Indre Finnmark" instead of an area.
</commit_message>
<xml_diff>
--- a/Data_AvailablityExp/spatiotemp_DataAvailability_Rype.xlsx
+++ b/Data_AvailablityExp/spatiotemp_DataAvailability_Rype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nina-my.sharepoint.com/personal/chloe_nater_nina_no/Documents/Documents/Projects/RypeDemografi/OpenPop_Integrated_DistSamp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nina-my.sharepoint.com/personal/chloe_nater_nina_no/Documents/Documents/Projects/RypeDemografi/OpenPop_Integrated_DistSamp/Data_AvailablityExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{87F498FB-BB24-4B51-94F0-2EC6F3816EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:40009_{87F498FB-BB24-4B51-94F0-2EC6F3816EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F46D273F-C943-4ED3-8466-05EEAFE02890}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="21740" windowHeight="9280" activeTab="1"/>
+    <workbookView xWindow="-4000" yWindow="1240" windowWidth="23910" windowHeight="11120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localities" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="172">
   <si>
     <t>dataSet</t>
   </si>
@@ -432,12 +432,117 @@
   </si>
   <si>
     <t>n_localities</t>
+  </si>
+  <si>
+    <t>FeFo</t>
+  </si>
+  <si>
+    <t>Indre Finnmark</t>
+  </si>
+  <si>
+    <t>Øst Finnmark</t>
+  </si>
+  <si>
+    <t>Vest Finnmark kyst</t>
+  </si>
+  <si>
+    <t>Anarjohka</t>
+  </si>
+  <si>
+    <t>Cunucearru</t>
+  </si>
+  <si>
+    <t>Geadgejavri</t>
+  </si>
+  <si>
+    <t>Karasjok Aitevarri</t>
+  </si>
+  <si>
+    <t>Karasjok Iskuras</t>
+  </si>
+  <si>
+    <t>Maze</t>
+  </si>
+  <si>
+    <t>Nattvann</t>
+  </si>
+  <si>
+    <t>Savngovann</t>
+  </si>
+  <si>
+    <t>Spielgajavrrit</t>
+  </si>
+  <si>
+    <t>Stalluvarre</t>
+  </si>
+  <si>
+    <t>Suossjavri</t>
+  </si>
+  <si>
+    <t>Blåsenborg</t>
+  </si>
+  <si>
+    <t>Byvann</t>
+  </si>
+  <si>
+    <t>Ifjord-Lebesby</t>
+  </si>
+  <si>
+    <t>Ifjord-Tana</t>
+  </si>
+  <si>
+    <t>Jarfjord</t>
+  </si>
+  <si>
+    <t>Komagdalen</t>
+  </si>
+  <si>
+    <t>Laksfjordvidda/Kunes</t>
+  </si>
+  <si>
+    <t>Maskevarre</t>
+  </si>
+  <si>
+    <t>Neiden</t>
+  </si>
+  <si>
+    <t>Nyborgmoen/Kroken</t>
+  </si>
+  <si>
+    <t>Pasvik</t>
+  </si>
+  <si>
+    <t>Tanadalen</t>
+  </si>
+  <si>
+    <t>Hatter</t>
+  </si>
+  <si>
+    <t>Hjelmsøy</t>
+  </si>
+  <si>
+    <t>Kjæs</t>
+  </si>
+  <si>
+    <t>Leirpollen</t>
+  </si>
+  <si>
+    <t>Rolvsøy</t>
+  </si>
+  <si>
+    <t>Sennalandet</t>
+  </si>
+  <si>
+    <t>Sørøya</t>
+  </si>
+  <si>
+    <t>Stilla – Joatka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -915,9 +1020,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1272,11 +1378,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2322,467 +2428,467 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="D40">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="E40">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="F40">
         <v>2020</v>
       </c>
       <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
         <v>14</v>
       </c>
-      <c r="H40">
-        <v>628</v>
+      <c r="I40" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="D41">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E41">
-        <v>2009</v>
+        <v>2000</v>
       </c>
       <c r="F41">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G41">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H41">
-        <v>496</v>
+        <v>542</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="D42">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E42">
         <v>2007</v>
       </c>
       <c r="F42">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G42">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H42">
-        <v>760</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43">
-        <v>2019</v>
+        <v>2009</v>
       </c>
       <c r="F43">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H43">
-        <v>7</v>
-      </c>
-      <c r="I43" t="s">
-        <v>134</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="D44">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E44">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="F44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G44">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H44">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E45">
-        <v>2019</v>
+        <v>2000</v>
       </c>
       <c r="F45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G45">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="H45">
-        <v>11</v>
-      </c>
-      <c r="I45" t="s">
-        <v>134</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>2013</v>
+      </c>
+      <c r="F46">
+        <v>2021</v>
+      </c>
+      <c r="G46">
         <v>9</v>
       </c>
-      <c r="E46">
-        <v>2006</v>
-      </c>
-      <c r="F46">
-        <v>2020</v>
-      </c>
-      <c r="G46">
-        <v>15</v>
-      </c>
       <c r="H46">
-        <v>343</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47">
-        <v>2019</v>
+        <v>2007</v>
       </c>
       <c r="F47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H47">
-        <v>15</v>
-      </c>
-      <c r="I47" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="D48">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="E48">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="F48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G48">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H48">
-        <v>194</v>
+        <v>349</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="D49">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E49">
-        <v>2009</v>
+        <v>2001</v>
       </c>
       <c r="F49">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="G49">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H49">
-        <v>436</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="D50">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E50">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="F50">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G50">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H50">
-        <v>1253</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="D51">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E51">
-        <v>2003</v>
+        <v>2007</v>
       </c>
       <c r="F51">
         <v>2020</v>
       </c>
       <c r="G51">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H51">
-        <v>5305</v>
+        <v>628</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52">
         <v>41</v>
       </c>
-      <c r="D52">
-        <v>13</v>
-      </c>
       <c r="E52">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="F52">
         <v>2020</v>
       </c>
       <c r="G52">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H52">
-        <v>1073</v>
+        <v>496</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D53">
         <v>26</v>
       </c>
       <c r="E53">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="F53">
         <v>2020</v>
       </c>
       <c r="G53">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H53">
-        <v>1436</v>
+        <v>760</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="D54">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E54">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="F54">
         <v>2020</v>
       </c>
       <c r="G54">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H54">
-        <v>159</v>
+        <v>7</v>
+      </c>
+      <c r="I54" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="D55">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E55">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F55">
         <v>2020</v>
       </c>
       <c r="G55">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H55">
-        <v>1416</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="D56">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E56">
-        <v>2007</v>
+        <v>2019</v>
       </c>
       <c r="F56">
         <v>2020</v>
       </c>
       <c r="G56">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H56">
-        <v>849</v>
+        <v>11</v>
+      </c>
+      <c r="I56" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="D57">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="E57">
         <v>2006</v>
@@ -2794,33 +2900,36 @@
         <v>15</v>
       </c>
       <c r="H57">
-        <v>1419</v>
+        <v>343</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C58" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="D58">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="E58">
-        <v>2006</v>
+        <v>2019</v>
       </c>
       <c r="F58">
         <v>2020</v>
       </c>
       <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
         <v>15</v>
       </c>
-      <c r="H58">
-        <v>2359</v>
+      <c r="I58" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -2828,652 +2937,652 @@
         <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C59" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D59">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="E59">
-        <v>2009</v>
+        <v>2015</v>
       </c>
       <c r="F59">
         <v>2020</v>
       </c>
       <c r="G59">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H59">
-        <v>1013</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="D60">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E60">
-        <v>2017</v>
+        <v>2009</v>
       </c>
       <c r="F60">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="G60">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H60">
-        <v>351</v>
+        <v>436</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="D61">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E61">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="F61">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="G61">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H61">
-        <v>817</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="C62" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E62">
-        <v>2011</v>
+        <v>2003</v>
       </c>
       <c r="F62">
         <v>2020</v>
       </c>
       <c r="G62">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H62">
-        <v>126</v>
+        <v>5305</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E63">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="F63">
         <v>2020</v>
       </c>
       <c r="G63">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H63">
-        <v>272</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="C64" t="s">
-        <v>110</v>
+        <v>42</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E64">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="F64">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="H64">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>39</v>
+      </c>
+      <c r="C65" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65">
         <v>12</v>
       </c>
-      <c r="I64" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" t="s">
-        <v>111</v>
-      </c>
-      <c r="D65">
-        <v>2</v>
-      </c>
       <c r="E65">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="F65">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G65">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H65">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="C66" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E66">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="F66">
         <v>2020</v>
       </c>
       <c r="G66">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H66">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="C67" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="D67">
         <v>9</v>
       </c>
       <c r="E67">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="F67">
         <v>2020</v>
       </c>
       <c r="G67">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H67">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="C68" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="D68">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="E68">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="F68">
         <v>2020</v>
       </c>
       <c r="G68">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H68">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="E69">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="F69">
         <v>2020</v>
       </c>
       <c r="G69">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H69">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C70" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="E70">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="F70">
         <v>2020</v>
       </c>
       <c r="G70">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H70">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E71">
-        <v>2011</v>
+        <v>2017</v>
       </c>
       <c r="F71">
         <v>2020</v>
       </c>
       <c r="G71">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H71">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="C72" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="D72">
         <v>18</v>
       </c>
       <c r="E72">
-        <v>2017</v>
+        <v>2007</v>
       </c>
       <c r="F72">
         <v>2020</v>
       </c>
       <c r="G72">
+        <v>14</v>
+      </c>
+      <c r="H72">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73">
         <v>4</v>
       </c>
-      <c r="H72">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>8</v>
-      </c>
-      <c r="B73" t="s">
-        <v>54</v>
-      </c>
-      <c r="C73" t="s">
-        <v>54</v>
-      </c>
-      <c r="D73">
+      <c r="E73">
+        <v>2011</v>
+      </c>
+      <c r="F73">
+        <v>2020</v>
+      </c>
+      <c r="G73">
+        <v>10</v>
+      </c>
+      <c r="H73">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>107</v>
+      </c>
+      <c r="C74" t="s">
+        <v>109</v>
+      </c>
+      <c r="D74">
+        <v>4</v>
+      </c>
+      <c r="E74">
+        <v>2011</v>
+      </c>
+      <c r="F74">
+        <v>2020</v>
+      </c>
+      <c r="G74">
+        <v>10</v>
+      </c>
+      <c r="H74">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>107</v>
+      </c>
+      <c r="C75" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>2011</v>
+      </c>
+      <c r="F75">
+        <v>2012</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="H75">
+        <v>12</v>
+      </c>
+      <c r="I75" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>2011</v>
+      </c>
+      <c r="F76">
+        <v>2019</v>
+      </c>
+      <c r="G76">
+        <v>9</v>
+      </c>
+      <c r="H76">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>2012</v>
+      </c>
+      <c r="F77">
+        <v>2020</v>
+      </c>
+      <c r="G77">
+        <v>9</v>
+      </c>
+      <c r="H77">
         <v>29</v>
       </c>
-      <c r="E73">
-        <v>2015</v>
-      </c>
-      <c r="F73">
-        <v>2020</v>
-      </c>
-      <c r="G73">
-        <v>6</v>
-      </c>
-      <c r="H73">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" t="s">
-        <v>55</v>
-      </c>
-      <c r="C74" t="s">
-        <v>55</v>
-      </c>
-      <c r="D74">
-        <v>18</v>
-      </c>
-      <c r="E74">
-        <v>2016</v>
-      </c>
-      <c r="F74">
-        <v>2020</v>
-      </c>
-      <c r="G74">
-        <v>5</v>
-      </c>
-      <c r="H74">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>8</v>
-      </c>
-      <c r="B75" t="s">
-        <v>56</v>
-      </c>
-      <c r="C75" t="s">
-        <v>57</v>
-      </c>
-      <c r="D75">
-        <v>9</v>
-      </c>
-      <c r="E75">
-        <v>2006</v>
-      </c>
-      <c r="F75">
-        <v>2020</v>
-      </c>
-      <c r="G75">
-        <v>15</v>
-      </c>
-      <c r="H75">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>8</v>
-      </c>
-      <c r="B76" t="s">
-        <v>58</v>
-      </c>
-      <c r="C76" t="s">
-        <v>59</v>
-      </c>
-      <c r="D76">
-        <v>25</v>
-      </c>
-      <c r="E76">
-        <v>2008</v>
-      </c>
-      <c r="F76">
-        <v>2020</v>
-      </c>
-      <c r="G76">
-        <v>13</v>
-      </c>
-      <c r="H76">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" t="s">
-        <v>58</v>
-      </c>
-      <c r="C77" t="s">
-        <v>60</v>
-      </c>
-      <c r="D77">
-        <v>32</v>
-      </c>
-      <c r="E77">
-        <v>2008</v>
-      </c>
-      <c r="F77">
-        <v>2020</v>
-      </c>
-      <c r="G77">
-        <v>13</v>
-      </c>
-      <c r="H77">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D78">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E78">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="F78">
         <v>2020</v>
       </c>
       <c r="G78">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H78">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B79" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="D79">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="E79">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="F79">
         <v>2020</v>
       </c>
       <c r="G79">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H79">
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B80" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="C80" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="D80">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="F80">
         <v>2020</v>
       </c>
       <c r="G80">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H80">
-        <v>547</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B81" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="C81" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="D81">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E81">
-        <v>2008</v>
+        <v>2011</v>
       </c>
       <c r="F81">
         <v>2020</v>
       </c>
       <c r="G81">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H81">
-        <v>1995</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="C82" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="D82">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="E82">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="F82">
         <v>2020</v>
       </c>
       <c r="G82">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H82">
-        <v>2509</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B83" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="D83">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E83">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F83">
         <v>2020</v>
       </c>
       <c r="G83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H83">
-        <v>834</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -3481,352 +3590,1167 @@
         <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C84" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D84">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E84">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="F84">
         <v>2020</v>
       </c>
       <c r="G84">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H84">
-        <v>1137</v>
+        <v>589</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="C85" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="D85">
-        <v>11</v>
-      </c>
-      <c r="E85">
-        <v>2012</v>
-      </c>
-      <c r="F85">
+        <v>18</v>
+      </c>
+      <c r="E85" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F85" s="2">
         <v>2020</v>
       </c>
       <c r="G85">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H85">
-        <v>104</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B86" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C86" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="D86">
-        <v>58</v>
-      </c>
-      <c r="E86">
-        <v>2014</v>
-      </c>
-      <c r="F86">
-        <v>2020</v>
+        <v>2</v>
+      </c>
+      <c r="E86" s="2">
+        <v>2008</v>
+      </c>
+      <c r="F86" s="2">
+        <v>2012</v>
       </c>
       <c r="G86">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H86">
-        <v>1512</v>
+        <v>10</v>
+      </c>
+      <c r="I86" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="B87" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="C87" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="D87">
-        <v>26</v>
-      </c>
-      <c r="E87">
-        <v>2007</v>
-      </c>
-      <c r="F87">
-        <v>2020</v>
+        <v>4</v>
+      </c>
+      <c r="E87" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F87" s="2">
+        <v>2021</v>
       </c>
       <c r="G87">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H87">
-        <v>1012</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="C88" t="s">
-        <v>71</v>
+        <v>154</v>
       </c>
       <c r="D88">
-        <v>20</v>
-      </c>
-      <c r="E88">
-        <v>2013</v>
-      </c>
-      <c r="F88">
-        <v>2020</v>
+        <v>2</v>
+      </c>
+      <c r="E88" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F88" s="2">
+        <v>2019</v>
       </c>
       <c r="G88">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H88">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="I88" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="C89" t="s">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="D89">
-        <v>27</v>
-      </c>
-      <c r="E89">
-        <v>2008</v>
-      </c>
-      <c r="F89">
-        <v>2020</v>
+        <v>2</v>
+      </c>
+      <c r="E89" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F89" s="2">
+        <v>2015</v>
       </c>
       <c r="G89">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H89">
-        <v>1581</v>
+        <v>14</v>
+      </c>
+      <c r="I89" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="B90" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="C90" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="D90">
-        <v>26</v>
-      </c>
-      <c r="E90">
-        <v>2009</v>
-      </c>
-      <c r="F90">
-        <v>2020</v>
+        <v>4</v>
+      </c>
+      <c r="E90" s="2">
+        <v>2011</v>
+      </c>
+      <c r="F90" s="2">
+        <v>2021</v>
       </c>
       <c r="G90">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H90">
-        <v>1117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="C91" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="D91">
-        <v>28</v>
-      </c>
-      <c r="E91">
-        <v>2009</v>
-      </c>
-      <c r="F91">
-        <v>2020</v>
+        <v>7</v>
+      </c>
+      <c r="E91" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F91" s="2">
+        <v>2021</v>
       </c>
       <c r="G91">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H91">
-        <v>611</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B92" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C92" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="D92">
-        <v>11</v>
-      </c>
-      <c r="E92">
-        <v>2014</v>
-      </c>
-      <c r="F92">
-        <v>2020</v>
+        <v>2</v>
+      </c>
+      <c r="E92" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F92" s="2">
+        <v>2021</v>
       </c>
       <c r="G92">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H92">
-        <v>468</v>
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B93" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C93" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="D93">
-        <v>3</v>
-      </c>
-      <c r="E93">
-        <v>2009</v>
-      </c>
-      <c r="F93">
-        <v>2012</v>
+        <v>2</v>
+      </c>
+      <c r="E93" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F93" s="2">
+        <v>2021</v>
       </c>
       <c r="G93">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="H93">
-        <v>14</v>
-      </c>
-      <c r="I93" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B94" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="D94">
-        <v>5</v>
-      </c>
-      <c r="E94">
-        <v>2009</v>
-      </c>
-      <c r="F94">
-        <v>2013</v>
+        <v>4</v>
+      </c>
+      <c r="E94" s="2">
+        <v>2012</v>
+      </c>
+      <c r="F94" s="2">
+        <v>2021</v>
       </c>
       <c r="G94">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H94">
-        <v>47</v>
-      </c>
-      <c r="I94" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B95" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C95" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="D95">
-        <v>13</v>
-      </c>
-      <c r="E95">
-        <v>2009</v>
-      </c>
-      <c r="F95">
-        <v>2020</v>
+        <v>10</v>
+      </c>
+      <c r="E95" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F95" s="2">
+        <v>2021</v>
       </c>
       <c r="G95">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H95">
-        <v>170</v>
+        <v>606</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>137</v>
+      </c>
+      <c r="B96" t="s">
+        <v>139</v>
+      </c>
+      <c r="C96" t="s">
+        <v>162</v>
+      </c>
+      <c r="D96">
+        <v>19</v>
+      </c>
+      <c r="E96" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F96" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G96">
+        <v>22</v>
+      </c>
+      <c r="H96">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>137</v>
+      </c>
+      <c r="B97" t="s">
+        <v>139</v>
+      </c>
+      <c r="C97" t="s">
+        <v>163</v>
+      </c>
+      <c r="D97">
+        <v>6</v>
+      </c>
+      <c r="E97" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F97" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G97">
+        <v>9</v>
+      </c>
+      <c r="H97">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" t="s">
+        <v>56</v>
+      </c>
+      <c r="C98" t="s">
+        <v>57</v>
+      </c>
+      <c r="D98">
+        <v>9</v>
+      </c>
+      <c r="E98">
+        <v>2006</v>
+      </c>
+      <c r="F98">
+        <v>2020</v>
+      </c>
+      <c r="G98">
+        <v>15</v>
+      </c>
+      <c r="H98">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" t="s">
+        <v>58</v>
+      </c>
+      <c r="C99" t="s">
+        <v>59</v>
+      </c>
+      <c r="D99">
+        <v>25</v>
+      </c>
+      <c r="E99">
+        <v>2008</v>
+      </c>
+      <c r="F99">
+        <v>2020</v>
+      </c>
+      <c r="G99">
+        <v>13</v>
+      </c>
+      <c r="H99">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100">
+        <v>32</v>
+      </c>
+      <c r="E100">
+        <v>2008</v>
+      </c>
+      <c r="F100">
+        <v>2020</v>
+      </c>
+      <c r="G100">
+        <v>13</v>
+      </c>
+      <c r="H100">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>74</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B101" t="s">
+        <v>119</v>
+      </c>
+      <c r="C101" t="s">
+        <v>119</v>
+      </c>
+      <c r="D101">
+        <v>12</v>
+      </c>
+      <c r="E101">
+        <v>2015</v>
+      </c>
+      <c r="F101">
+        <v>2020</v>
+      </c>
+      <c r="G101">
+        <v>6</v>
+      </c>
+      <c r="H101">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" t="s">
+        <v>61</v>
+      </c>
+      <c r="C102" t="s">
+        <v>61</v>
+      </c>
+      <c r="D102">
+        <v>48</v>
+      </c>
+      <c r="E102">
+        <v>2006</v>
+      </c>
+      <c r="F102">
+        <v>2020</v>
+      </c>
+      <c r="G102">
+        <v>15</v>
+      </c>
+      <c r="H102">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" t="s">
+        <v>62</v>
+      </c>
+      <c r="C103" t="s">
+        <v>62</v>
+      </c>
+      <c r="D103">
+        <v>22</v>
+      </c>
+      <c r="E103">
+        <v>2018</v>
+      </c>
+      <c r="F103">
+        <v>2020</v>
+      </c>
+      <c r="G103">
+        <v>3</v>
+      </c>
+      <c r="H103">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" t="s">
+        <v>63</v>
+      </c>
+      <c r="C104" t="s">
+        <v>63</v>
+      </c>
+      <c r="D104">
+        <v>37</v>
+      </c>
+      <c r="E104">
+        <v>2008</v>
+      </c>
+      <c r="F104">
+        <v>2020</v>
+      </c>
+      <c r="G104">
+        <v>13</v>
+      </c>
+      <c r="H104">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" t="s">
+        <v>64</v>
+      </c>
+      <c r="C105" t="s">
+        <v>64</v>
+      </c>
+      <c r="D105">
+        <v>48</v>
+      </c>
+      <c r="E105">
+        <v>2006</v>
+      </c>
+      <c r="F105">
+        <v>2020</v>
+      </c>
+      <c r="G105">
+        <v>15</v>
+      </c>
+      <c r="H105">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" t="s">
+        <v>66</v>
+      </c>
+      <c r="D106">
+        <v>22</v>
+      </c>
+      <c r="E106">
+        <v>2016</v>
+      </c>
+      <c r="F106">
+        <v>2020</v>
+      </c>
+      <c r="G106">
+        <v>5</v>
+      </c>
+      <c r="H106">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" t="s">
+        <v>67</v>
+      </c>
+      <c r="C107" t="s">
+        <v>68</v>
+      </c>
+      <c r="D107">
+        <v>38</v>
+      </c>
+      <c r="E107">
+        <v>2010</v>
+      </c>
+      <c r="F107">
+        <v>2020</v>
+      </c>
+      <c r="G107">
+        <v>11</v>
+      </c>
+      <c r="H107">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>74</v>
+      </c>
+      <c r="B108" t="s">
+        <v>120</v>
+      </c>
+      <c r="C108" t="s">
+        <v>120</v>
+      </c>
+      <c r="D108">
+        <v>11</v>
+      </c>
+      <c r="E108">
+        <v>2012</v>
+      </c>
+      <c r="F108">
+        <v>2020</v>
+      </c>
+      <c r="G108">
+        <v>9</v>
+      </c>
+      <c r="H108">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>74</v>
+      </c>
+      <c r="B109" t="s">
+        <v>121</v>
+      </c>
+      <c r="C109" t="s">
+        <v>121</v>
+      </c>
+      <c r="D109">
+        <v>58</v>
+      </c>
+      <c r="E109">
+        <v>2014</v>
+      </c>
+      <c r="F109">
+        <v>2020</v>
+      </c>
+      <c r="G109">
+        <v>7</v>
+      </c>
+      <c r="H109">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" t="s">
+        <v>69</v>
+      </c>
+      <c r="C110" t="s">
+        <v>70</v>
+      </c>
+      <c r="D110">
+        <v>26</v>
+      </c>
+      <c r="E110">
+        <v>2007</v>
+      </c>
+      <c r="F110">
+        <v>2020</v>
+      </c>
+      <c r="G110">
+        <v>14</v>
+      </c>
+      <c r="H110">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" t="s">
+        <v>69</v>
+      </c>
+      <c r="C111" t="s">
+        <v>71</v>
+      </c>
+      <c r="D111">
+        <v>20</v>
+      </c>
+      <c r="E111">
+        <v>2013</v>
+      </c>
+      <c r="F111">
+        <v>2020</v>
+      </c>
+      <c r="G111">
+        <v>8</v>
+      </c>
+      <c r="H111">
+        <v>159</v>
+      </c>
+      <c r="I111" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" t="s">
+        <v>72</v>
+      </c>
+      <c r="C112" t="s">
+        <v>72</v>
+      </c>
+      <c r="D112">
+        <v>27</v>
+      </c>
+      <c r="E112">
+        <v>2008</v>
+      </c>
+      <c r="F112">
+        <v>2020</v>
+      </c>
+      <c r="G112">
+        <v>13</v>
+      </c>
+      <c r="H112">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>137</v>
+      </c>
+      <c r="B113" t="s">
+        <v>140</v>
+      </c>
+      <c r="C113" t="s">
+        <v>164</v>
+      </c>
+      <c r="D113">
+        <v>4</v>
+      </c>
+      <c r="E113" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F113" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G113">
+        <v>9</v>
+      </c>
+      <c r="H113">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>137</v>
+      </c>
+      <c r="B114" t="s">
+        <v>140</v>
+      </c>
+      <c r="C114" t="s">
+        <v>165</v>
+      </c>
+      <c r="D114">
+        <v>4</v>
+      </c>
+      <c r="E114" s="2">
+        <v>2012</v>
+      </c>
+      <c r="F114" s="2">
+        <v>2020</v>
+      </c>
+      <c r="G114">
+        <v>9</v>
+      </c>
+      <c r="H114">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>137</v>
+      </c>
+      <c r="B115" t="s">
+        <v>140</v>
+      </c>
+      <c r="C115" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115">
+        <v>45</v>
+      </c>
+      <c r="E115" s="2">
+        <v>2008</v>
+      </c>
+      <c r="F115" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G115">
+        <v>14</v>
+      </c>
+      <c r="H115">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>137</v>
+      </c>
+      <c r="B116" t="s">
+        <v>140</v>
+      </c>
+      <c r="C116" t="s">
+        <v>167</v>
+      </c>
+      <c r="D116">
+        <v>37</v>
+      </c>
+      <c r="E116" s="2">
+        <v>2007</v>
+      </c>
+      <c r="F116" s="2">
+        <v>2012</v>
+      </c>
+      <c r="G116">
+        <v>6</v>
+      </c>
+      <c r="H116">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>137</v>
+      </c>
+      <c r="B117" t="s">
+        <v>140</v>
+      </c>
+      <c r="C117" t="s">
+        <v>168</v>
+      </c>
+      <c r="D117">
+        <v>4</v>
+      </c>
+      <c r="E117" s="2">
+        <v>2012</v>
+      </c>
+      <c r="F117" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G117">
+        <v>10</v>
+      </c>
+      <c r="H117">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>137</v>
+      </c>
+      <c r="B118" t="s">
+        <v>140</v>
+      </c>
+      <c r="C118" t="s">
+        <v>169</v>
+      </c>
+      <c r="D118">
+        <v>12</v>
+      </c>
+      <c r="E118" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F118" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G118">
+        <v>22</v>
+      </c>
+      <c r="H118">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>137</v>
+      </c>
+      <c r="B119" t="s">
+        <v>140</v>
+      </c>
+      <c r="C119" t="s">
+        <v>170</v>
+      </c>
+      <c r="D119">
+        <v>6</v>
+      </c>
+      <c r="E119" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F119" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G119">
+        <v>22</v>
+      </c>
+      <c r="H119">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>137</v>
+      </c>
+      <c r="B120" t="s">
+        <v>140</v>
+      </c>
+      <c r="C120" t="s">
+        <v>171</v>
+      </c>
+      <c r="D120">
+        <v>12</v>
+      </c>
+      <c r="E120" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F120" s="2">
+        <v>2021</v>
+      </c>
+      <c r="G120">
+        <v>22</v>
+      </c>
+      <c r="H120">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>8</v>
+      </c>
+      <c r="B121" t="s">
+        <v>73</v>
+      </c>
+      <c r="C121" t="s">
+        <v>73</v>
+      </c>
+      <c r="D121">
+        <v>26</v>
+      </c>
+      <c r="E121">
+        <v>2009</v>
+      </c>
+      <c r="F121">
+        <v>2020</v>
+      </c>
+      <c r="G121">
+        <v>12</v>
+      </c>
+      <c r="H121">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>74</v>
+      </c>
+      <c r="B122" t="s">
+        <v>122</v>
+      </c>
+      <c r="C122" t="s">
+        <v>122</v>
+      </c>
+      <c r="D122">
+        <v>28</v>
+      </c>
+      <c r="E122">
+        <v>2009</v>
+      </c>
+      <c r="F122">
+        <v>2020</v>
+      </c>
+      <c r="G122">
+        <v>12</v>
+      </c>
+      <c r="H122">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>74</v>
+      </c>
+      <c r="B123" t="s">
         <v>123</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C123" t="s">
+        <v>124</v>
+      </c>
+      <c r="D123">
+        <v>11</v>
+      </c>
+      <c r="E123">
+        <v>2014</v>
+      </c>
+      <c r="F123">
+        <v>2020</v>
+      </c>
+      <c r="G123">
+        <v>7</v>
+      </c>
+      <c r="H123">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>74</v>
+      </c>
+      <c r="B124" t="s">
+        <v>123</v>
+      </c>
+      <c r="C124" t="s">
+        <v>125</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
+      </c>
+      <c r="E124">
+        <v>2009</v>
+      </c>
+      <c r="F124">
+        <v>2012</v>
+      </c>
+      <c r="G124">
+        <v>4</v>
+      </c>
+      <c r="H124">
+        <v>14</v>
+      </c>
+      <c r="I124" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>74</v>
+      </c>
+      <c r="B125" t="s">
+        <v>123</v>
+      </c>
+      <c r="C125" t="s">
+        <v>126</v>
+      </c>
+      <c r="D125">
+        <v>5</v>
+      </c>
+      <c r="E125">
+        <v>2009</v>
+      </c>
+      <c r="F125">
+        <v>2013</v>
+      </c>
+      <c r="G125">
+        <v>5</v>
+      </c>
+      <c r="H125">
+        <v>47</v>
+      </c>
+      <c r="I125" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>74</v>
+      </c>
+      <c r="B126" t="s">
+        <v>123</v>
+      </c>
+      <c r="C126" t="s">
+        <v>127</v>
+      </c>
+      <c r="D126">
+        <v>13</v>
+      </c>
+      <c r="E126">
+        <v>2009</v>
+      </c>
+      <c r="F126">
+        <v>2020</v>
+      </c>
+      <c r="G126">
+        <v>12</v>
+      </c>
+      <c r="H126">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>74</v>
+      </c>
+      <c r="B127" t="s">
+        <v>123</v>
+      </c>
+      <c r="C127" t="s">
         <v>128</v>
       </c>
-      <c r="D96">
+      <c r="D127">
         <v>14</v>
       </c>
-      <c r="E96">
+      <c r="E127">
         <v>2008</v>
       </c>
-      <c r="F96">
-        <v>2020</v>
-      </c>
-      <c r="G96">
+      <c r="F127">
+        <v>2020</v>
+      </c>
+      <c r="G127">
         <v>13</v>
       </c>
-      <c r="H96">
+      <c r="H127">
         <v>504</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J96">
-    <sortCondition ref="B2:B96"/>
-    <sortCondition ref="C2:C96"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J127">
+    <sortCondition ref="B2:B127"/>
+    <sortCondition ref="C2:C127"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3834,11 +4758,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5076,6 +6000,93 @@
         <v>1203</v>
       </c>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43">
+        <v>11</v>
+      </c>
+      <c r="E43">
+        <v>126</v>
+      </c>
+      <c r="F43">
+        <v>2000</v>
+      </c>
+      <c r="G43">
+        <v>2021</v>
+      </c>
+      <c r="H43">
+        <v>22</v>
+      </c>
+      <c r="I43">
+        <v>2734</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+      <c r="E44">
+        <v>64</v>
+      </c>
+      <c r="F44">
+        <v>2000</v>
+      </c>
+      <c r="G44">
+        <v>2021</v>
+      </c>
+      <c r="H44">
+        <v>22</v>
+      </c>
+      <c r="I44">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <v>124</v>
+      </c>
+      <c r="F45">
+        <v>2000</v>
+      </c>
+      <c r="G45">
+        <v>2021</v>
+      </c>
+      <c r="H45">
+        <v>22</v>
+      </c>
+      <c r="I45">
+        <v>3497</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>